<commit_message>
Ran some more experiments and saved their results. Also fine tuned MobileNet on 20 and 30 epochs and saved the weights.
</commit_message>
<xml_diff>
--- a/Fine Tuning Results/Fine Tuning Results.xlsx
+++ b/Fine Tuning Results/Fine Tuning Results.xlsx
@@ -18,8 +18,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Froze the CNN part and trained custom classifier.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Froze the CNN part and trained custom classifier.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Model</t>
   </si>
@@ -39,9 +97,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>bce</t>
   </si>
   <si>
@@ -115,13 +170,16 @@
   </si>
   <si>
     <t>Nod</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +194,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -448,11 +519,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,85 +562,85 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:30" x14ac:dyDescent="0.3">
@@ -598,11 +669,9 @@
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="3">
         <v>75.7</v>
       </c>
@@ -665,67 +734,175 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1">
+        <v>224</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
+      <c r="L3" s="3">
+        <v>75.7</v>
+      </c>
+      <c r="M3" s="1">
+        <v>49.8</v>
+      </c>
+      <c r="N3" s="1">
+        <v>51</v>
+      </c>
+      <c r="O3" s="1">
+        <v>52.3</v>
+      </c>
+      <c r="P3" s="1">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>68</v>
+      </c>
+      <c r="R3" s="1">
+        <v>75</v>
+      </c>
+      <c r="S3" s="1">
+        <v>70</v>
+      </c>
+      <c r="T3" s="1">
+        <v>87</v>
+      </c>
+      <c r="U3" s="1">
+        <v>84</v>
+      </c>
+      <c r="V3" s="1">
+        <v>64</v>
+      </c>
+      <c r="W3" s="1">
+        <v>82</v>
+      </c>
+      <c r="X3" s="1">
+        <v>77</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>79</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>73</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>76</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>67</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>81</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>72</v>
+      </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1">
+        <v>39.6</v>
+      </c>
+      <c r="F4" s="1">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1">
+        <v>224</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="K4" s="1"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
+      <c r="L4" s="3">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="M4" s="1">
+        <v>61.8</v>
+      </c>
+      <c r="N4" s="1">
+        <v>50</v>
+      </c>
+      <c r="O4" s="1">
+        <v>41.7</v>
+      </c>
+      <c r="P4" s="1">
+        <v>79</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>70</v>
+      </c>
+      <c r="R4" s="1">
+        <v>75</v>
+      </c>
+      <c r="S4" s="1">
+        <v>70</v>
+      </c>
+      <c r="T4" s="1">
+        <v>88</v>
+      </c>
+      <c r="U4" s="1">
+        <v>83</v>
+      </c>
+      <c r="V4" s="1">
+        <v>65</v>
+      </c>
+      <c r="W4" s="1">
+        <v>83</v>
+      </c>
+      <c r="X4" s="1">
+        <v>77</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>80</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>73</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>77</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>67</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>81</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>73</v>
+      </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5">
@@ -1660,5 +1837,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>